<commit_message>
merged data and performance in euro
</commit_message>
<xml_diff>
--- a/wartosci_walorow_dane_zrodlowe.xlsx
+++ b/wartosci_walorow_dane_zrodlowe.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja portfela\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEEA5233-3DB6-49D2-BC74-D8C073DE742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A80C7C-D7E0-4D21-8EB4-824B096FA2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSCI EM" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="swig80tr_m" sheetId="13" r:id="rId14"/>
     <sheet name="swig80_m" sheetId="12" r:id="rId15"/>
     <sheet name="wig20tr_m" sheetId="11" r:id="rId16"/>
-    <sheet name="wartości indeksów - dane źródło" sheetId="21" r:id="rId17"/>
+    <sheet name="Gold" sheetId="21" r:id="rId17"/>
     <sheet name="wig20" sheetId="10" r:id="rId18"/>
   </sheets>
   <definedNames>
@@ -38,9 +38,9 @@
     <definedName name="DaneZewnętrzne_1" localSheetId="17" hidden="1">'wig20'!$A$1:$D$250</definedName>
     <definedName name="DaneZewnętrzne_2" localSheetId="6" hidden="1">'AGG BOND'!$A$1:$B$99</definedName>
     <definedName name="DaneZewnętrzne_2" localSheetId="9" hidden="1">'GLOBAL CORP'!$A$1:$B$117</definedName>
+    <definedName name="DaneZewnętrzne_2" localSheetId="16" hidden="1">Gold!$A$1:$B$522</definedName>
     <definedName name="DaneZewnętrzne_2" localSheetId="12" hidden="1">mwig40_m!$A$1:$C$258</definedName>
     <definedName name="DaneZewnętrzne_2" localSheetId="4" hidden="1">'SP500'!$A$1:$B$364</definedName>
-    <definedName name="DaneZewnętrzne_2" localSheetId="16" hidden="1">'wartości indeksów - dane źródło'!$A$1:$B$522</definedName>
     <definedName name="DaneZewnętrzne_2" localSheetId="15" hidden="1">wig20tr_m!$A$1:$D$212</definedName>
     <definedName name="DaneZewnętrzne_3" localSheetId="8" hidden="1">'^tbsp_m(1)'!$A$1:$C$188</definedName>
     <definedName name="DaneZewnętrzne_3" localSheetId="3" hidden="1">'MSCI EUROPE'!$A$1:$B$522</definedName>
@@ -51,61 +51,73 @@
     <definedName name="DaneZewnętrzne_5" localSheetId="1" hidden="1">'MSCI Japan'!$A$1:$B$522</definedName>
     <definedName name="DaneZewnętrzne_6" localSheetId="0" hidden="1">'MSCI EM'!$A$1:$B$414</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Zapytanie — ^tbsp_m(1)" description="Połączenie z zapytaniem „^tbsp_m(1)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Zapytanie — ^tbsp_m(1)" description="Połączenie z zapytaniem „^tbsp_m(1)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=^tbsp_m(1);Extended Properties=&quot;&quot;" command="SELECT * FROM [^tbsp_m(1)]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Zapytanie — chart(10)" description="Połączenie z zapytaniem „chart(10)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Zapytanie — chart(10)" description="Połączenie z zapytaniem „chart(10)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(10);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(10)]"/>
   </connection>
-  <connection id="3" keepAlive="1" name="Zapytanie — chart(11)" description="Połączenie z zapytaniem „chart(11)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" keepAlive="1" name="Zapytanie — chart(11)" description="Połączenie z zapytaniem „chart(11)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(11);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(11)]"/>
   </connection>
-  <connection id="4" keepAlive="1" name="Zapytanie — chart(12)" description="Połączenie z zapytaniem „chart(12)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" keepAlive="1" name="Zapytanie — chart(12)" description="Połączenie z zapytaniem „chart(12)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(12);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(12)]"/>
   </connection>
-  <connection id="5" keepAlive="1" name="Zapytanie — chart(13)" description="Połączenie z zapytaniem „chart(13)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" keepAlive="1" name="Zapytanie — chart(13)" description="Połączenie z zapytaniem „chart(13)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(13);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(13)]"/>
   </connection>
-  <connection id="6" keepAlive="1" name="Zapytanie — chart(14)" description="Połączenie z zapytaniem „chart(14)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" keepAlive="1" name="Zapytanie — chart(14)" description="Połączenie z zapytaniem „chart(14)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(14);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(14)]"/>
   </connection>
-  <connection id="7" keepAlive="1" name="Zapytanie — chart(5)" description="Połączenie z zapytaniem „chart(5)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" keepAlive="1" name="Zapytanie — chart(5)" description="Połączenie z zapytaniem „chart(5)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(5);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(5)]"/>
   </connection>
-  <connection id="8" keepAlive="1" name="Zapytanie — chart(6)" description="Połączenie z zapytaniem „chart(6)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" keepAlive="1" name="Zapytanie — chart(6)" description="Połączenie z zapytaniem „chart(6)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(6);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(6)]"/>
   </connection>
-  <connection id="9" keepAlive="1" name="Zapytanie — chart(7)" description="Połączenie z zapytaniem „chart(7)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" keepAlive="1" name="Zapytanie — chart(7)" description="Połączenie z zapytaniem „chart(7)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(7);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(7)]"/>
   </connection>
-  <connection id="10" keepAlive="1" name="Zapytanie — chart(8)" description="Połączenie z zapytaniem „chart(8)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" keepAlive="1" name="Zapytanie — chart(8)" description="Połączenie z zapytaniem „chart(8)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(8);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(8)]"/>
   </connection>
-  <connection id="11" keepAlive="1" name="Zapytanie — chart(9)" description="Połączenie z zapytaniem „chart(9)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" keepAlive="1" name="Zapytanie — chart(9)" description="Połączenie z zapytaniem „chart(9)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=chart(9);Extended Properties=&quot;&quot;" command="SELECT * FROM [chart(9)]"/>
   </connection>
-  <connection id="12" keepAlive="1" name="Zapytanie — eurpln_m" description="Połączenie z zapytaniem „eurpln_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" keepAlive="1" name="Zapytanie — eurpln_m" description="Połączenie z zapytaniem „eurpln_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=eurpln_m;Extended Properties=&quot;&quot;" command="SELECT * FROM [eurpln_m]"/>
   </connection>
-  <connection id="13" keepAlive="1" name="Zapytanie — mwig40_m" description="Połączenie z zapytaniem „mwig40_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF0C000000}" keepAlive="1" name="Zapytanie — mwig40_m" description="Połączenie z zapytaniem „mwig40_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=mwig40_m;Extended Properties=&quot;&quot;" command="SELECT * FROM [mwig40_m]"/>
   </connection>
-  <connection id="14" keepAlive="1" name="Zapytanie — swig80_m" description="Połączenie z zapytaniem „swig80_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="14" xr16:uid="{00000000-0015-0000-FFFF-FFFF0D000000}" keepAlive="1" name="Zapytanie — swig80_m" description="Połączenie z zapytaniem „swig80_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=swig80_m;Extended Properties=&quot;&quot;" command="SELECT * FROM [swig80_m]"/>
   </connection>
-  <connection id="15" keepAlive="1" name="Zapytanie — swig80tr_m" description="Połączenie z zapytaniem „swig80tr_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="15" xr16:uid="{00000000-0015-0000-FFFF-FFFF0E000000}" keepAlive="1" name="Zapytanie — swig80tr_m" description="Połączenie z zapytaniem „swig80tr_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=swig80tr_m;Extended Properties=&quot;&quot;" command="SELECT * FROM [swig80tr_m]"/>
   </connection>
-  <connection id="16" keepAlive="1" name="Zapytanie — wig20_m(1)" description="Połączenie z zapytaniem „wig20_m(1)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="16" xr16:uid="{00000000-0015-0000-FFFF-FFFF0F000000}" keepAlive="1" name="Zapytanie — wig20_m(1)" description="Połączenie z zapytaniem „wig20_m(1)” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=wig20_m(1);Extended Properties=&quot;&quot;" command="SELECT * FROM [wig20_m(1)]"/>
   </connection>
-  <connection id="17" keepAlive="1" name="Zapytanie — wig20tr_m" description="Połączenie z zapytaniem „wig20tr_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="17" xr16:uid="{00000000-0015-0000-FFFF-FFFF10000000}" keepAlive="1" name="Zapytanie — wig20tr_m" description="Połączenie z zapytaniem „wig20tr_m” w skoroszycie." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=wig20tr_m;Extended Properties=&quot;&quot;" command="SELECT * FROM [wig20tr_m]"/>
   </connection>
 </connections>
@@ -255,7 +267,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,13 +877,49 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -891,37 +939,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -934,13 +951,7 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -968,6 +979,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1040,7 +1052,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_6" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_6" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1052,7 +1064,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_2" connectionId="5" xr16:uid="{00000000-0016-0000-0900-000009000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1064,7 +1076,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_1" connectionId="3" xr16:uid="{00000000-0016-0000-0A00-00000A000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1076,7 +1088,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_2" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_2" connectionId="13" xr16:uid="{00000000-0016-0000-0C00-00000B000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="12" unboundColumnsRight="1">
     <queryTableFields count="4">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1095,7 +1107,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_4" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_4" connectionId="15" xr16:uid="{00000000-0016-0000-0D00-00000C000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1113,7 +1125,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_3" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_3" connectionId="14" xr16:uid="{00000000-0016-0000-0E00-00000D000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="9">
     <queryTableFields count="4">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1131,7 +1143,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_2" connectionId="17" xr16:uid="{00000000-0016-0000-0F00-00000E000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1149,7 +1161,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_2" connectionId="6" xr16:uid="{00000000-0016-0000-1000-00000F000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1161,7 +1173,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_1" connectionId="16" xr16:uid="{00000000-0016-0000-1100-000010000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
     <queryTableFields count="4">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1179,7 +1191,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_5" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_5" connectionId="11" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1191,7 +1203,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_4" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_4" connectionId="10" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1203,7 +1215,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_3" connectionId="9" xr16:uid="{00000000-0016-0000-0300-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1215,7 +1227,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_2" connectionId="8" xr16:uid="{00000000-0016-0000-0400-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1227,7 +1239,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_1" connectionId="7" xr16:uid="{00000000-0016-0000-0500-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1239,7 +1251,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_2" connectionId="4" xr16:uid="{00000000-0016-0000-0600-000006000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Date" tableColumnId="1"/>
@@ -1251,7 +1263,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_4" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_4" connectionId="12" xr16:uid="{00000000-0016-0000-0700-000007000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7" unboundColumnsRight="1">
     <queryTableFields count="3">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1268,7 +1280,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DaneZewnętrzne_3" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DaneZewnętrzne_3" connectionId="1" xr16:uid="{00000000-0016-0000-0800-000008000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
     <queryTableFields count="3">
       <queryTableField id="1" name="Data" tableColumnId="1"/>
@@ -1285,12 +1297,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="chart_10" displayName="chart_10" ref="A1:C414" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C414"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="chart_10" displayName="chart_10" ref="A1:C414" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C414" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="37"/>
-    <tableColumn id="2" uniqueName="2" name="MSCI Emerging Markets" queryTableFieldId="2" dataDxfId="36"/>
-    <tableColumn id="3" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="35" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="MSCI Emerging Markets" queryTableFieldId="2" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="50" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_10[[#This Row],[MSCI Emerging Markets]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1299,12 +1311,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="chart_13" displayName="chart_13" ref="A1:C117" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="chart_13" displayName="chart_13" ref="A1:C117" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C117" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="15"/>
-    <tableColumn id="2" uniqueName="2" name="Bloomberg Barclays Global Aggregate Corporate" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="3" uniqueName="3" name="Zmiany miesięczne" queryTableFieldId="3" dataDxfId="8" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" uniqueName="2" name="Bloomberg Barclays Global Aggregate Corporate" queryTableFieldId="2" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" uniqueName="3" name="Zmiany miesięczne" queryTableFieldId="3" dataDxfId="24" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_13[[#This Row],[Bloomberg Barclays Global Aggregate Corporate]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1313,12 +1325,12 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="chart_11" displayName="chart_11" ref="A1:C99" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="chart_11" displayName="chart_11" ref="A1:C99" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C99" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="21"/>
-    <tableColumn id="2" uniqueName="2" name="Bloomberg Barclays Global Aggregate Bond (Hedged EUR)" queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="3" uniqueName="3" name="zmiana miesieczna" queryTableFieldId="3" dataDxfId="19" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" uniqueName="2" name="Bloomberg Barclays Global Aggregate Bond (Hedged EUR)" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" uniqueName="3" name="zmiana miesieczna" queryTableFieldId="3" dataDxfId="21" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_11[[#This Row],[Bloomberg Barclays Global Aggregate Bond (Hedged EUR)]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1327,13 +1339,13 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="mwig40_m" displayName="mwig40_m" ref="A1:D258" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D258"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="mwig40_m" displayName="mwig40_m" ref="A1:D258" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D258" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="34"/>
-    <tableColumn id="11" uniqueName="11" name="Data" queryTableFieldId="11" dataDxfId="7"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="33"/>
-    <tableColumn id="10" uniqueName="10" name="Zmiana miesięczna" queryTableFieldId="10" dataDxfId="32" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0B00-00000B000000}" uniqueName="11" name="Data" queryTableFieldId="11" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" uniqueName="10" name="Zmiana miesięczna" queryTableFieldId="10" dataDxfId="17" dataCellStyle="Procentowy">
       <calculatedColumnFormula>mwig40_m[[#This Row],[Zamkniecie]]/C1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1342,51 +1354,51 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="swig80tr_m" displayName="swig80tr_m" ref="A1:D152" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D152"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="swig80tr_m" displayName="swig80tr_m" ref="A1:D152" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D152" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="24"/>
-    <tableColumn id="7" uniqueName="7" name="Data" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="23"/>
-    <tableColumn id="6" uniqueName="6" name="Zmiana miesięczna" queryTableFieldId="6" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" uniqueName="7" name="Data" queryTableFieldId="7" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" uniqueName="6" name="Zmiana miesięczna" queryTableFieldId="6" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="swig80_m" displayName="swig80_m" ref="A1:D250" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D250"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="swig80_m" displayName="swig80_m" ref="A1:D250" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D250" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="26"/>
-    <tableColumn id="7" uniqueName="7" name="Data" queryTableFieldId="7" dataDxfId="6"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="25"/>
-    <tableColumn id="6" uniqueName="6" name="Kolumna1" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" uniqueName="7" name="Data" queryTableFieldId="7" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" uniqueName="6" name="Kolumna1" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="wig20tr_m" displayName="wig20tr_m" ref="A1:D212" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D212"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="wig20tr_m" displayName="wig20tr_m" ref="A1:D212" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D212" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Data" queryTableFieldId="1" dataDxfId="28"/>
-    <tableColumn id="7" uniqueName="7" name="Kolumna1" queryTableFieldId="7" dataDxfId="5"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="27"/>
-    <tableColumn id="6" uniqueName="6" name="Zmiana miesięczna" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" uniqueName="1" name="Data" queryTableFieldId="1" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" uniqueName="7" name="Kolumna1" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" uniqueName="6" name="Zmiana miesięczna" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="chart_14" displayName="chart_14" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C522"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="chart_14" displayName="chart_14" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C522" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="2" uniqueName="2" name="Gold spot price" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="0" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" uniqueName="2" name="Gold spot price" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="4" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_14[[#This Row],[Gold spot price]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1395,25 +1407,25 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="wig20_m_1" displayName="wig20_m_1" ref="A1:D250" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D250"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="wig20_m_1" displayName="wig20_m_1" ref="A1:D250" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D250" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="31"/>
-    <tableColumn id="7" uniqueName="7" name="Data" queryTableFieldId="7" dataDxfId="3"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="30"/>
-    <tableColumn id="6" uniqueName="6" name="Zmiana miesięczna" queryTableFieldId="6" dataDxfId="29" dataCellStyle="Procentowy"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" uniqueName="1" name="Data oryginalna" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" uniqueName="7" name="Data" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" uniqueName="6" name="Zmiana miesięczna" queryTableFieldId="6" dataDxfId="0" dataCellStyle="Procentowy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="chart_9" displayName="chart_9" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C522"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="chart_9" displayName="chart_9" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C522" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="40"/>
-    <tableColumn id="2" uniqueName="2" name="MSCI Japan" queryTableFieldId="2" dataDxfId="39"/>
-    <tableColumn id="3" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="38" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="2" name="MSCI Japan" queryTableFieldId="2" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="47" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_9[[#This Row],[MSCI Japan]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1422,12 +1434,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="chart_8" displayName="chart_8" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C522"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="chart_8" displayName="chart_8" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C522" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="43"/>
-    <tableColumn id="2" uniqueName="2" name="MSCI Pacific ex-Japan" queryTableFieldId="2" dataDxfId="42"/>
-    <tableColumn id="3" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="41" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" uniqueName="2" name="MSCI Pacific ex-Japan" queryTableFieldId="2" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="44" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_8[[#This Row],[MSCI Pacific ex-Japan]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1436,12 +1448,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="chart_7" displayName="chart_7" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C522"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="chart_7" displayName="chart_7" ref="A1:C522" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C522" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="46"/>
-    <tableColumn id="2" uniqueName="2" name="MSCI Europe" queryTableFieldId="2" dataDxfId="45"/>
-    <tableColumn id="3" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="44" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" uniqueName="2" name="MSCI Europe" queryTableFieldId="2" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="41" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_7[[#This Row],[MSCI Europe]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1450,12 +1462,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="chart_6" displayName="chart_6" ref="A1:C364" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C364"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="chart_6" displayName="chart_6" ref="A1:C364" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C364" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="49"/>
-    <tableColumn id="2" uniqueName="2" name="S&amp;P 500" queryTableFieldId="2" dataDxfId="48"/>
-    <tableColumn id="3" uniqueName="3" name="S&amp;P 501" queryTableFieldId="3" dataDxfId="47" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" uniqueName="2" name="S&amp;P 500" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" uniqueName="3" name="S&amp;P 501" queryTableFieldId="3" dataDxfId="38" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_6[[#This Row],[S&amp;P 500]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1464,12 +1476,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="chart_5" displayName="chart_5" ref="A1:C414" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C414"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="chart_5" displayName="chart_5" ref="A1:C414" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C414" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="52"/>
-    <tableColumn id="2" uniqueName="2" name="MSCI ACWI" queryTableFieldId="2" dataDxfId="51"/>
-    <tableColumn id="3" uniqueName="3" name="Zmiany miesięczne" queryTableFieldId="3" dataDxfId="50" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" uniqueName="2" name="MSCI ACWI" queryTableFieldId="2" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" uniqueName="3" name="Zmiany miesięczne" queryTableFieldId="3" dataDxfId="35" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_5[[#This Row],[MSCI ACWI]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1478,12 +1490,12 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="chart_12" displayName="chart_12" ref="A1:C99" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="chart_12" displayName="chart_12" ref="A1:C99" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C99" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="18"/>
-    <tableColumn id="2" uniqueName="2" name="Bloomberg Barclays Global Aggregate Bond" queryTableFieldId="2" dataDxfId="17"/>
-    <tableColumn id="3" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="16" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" uniqueName="2" name="Bloomberg Barclays Global Aggregate Bond" queryTableFieldId="2" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" uniqueName="3" name="Kolumna1" queryTableFieldId="3" dataDxfId="32" dataCellStyle="Procentowy">
       <calculatedColumnFormula>chart_12[[#This Row],[Bloomberg Barclays Global Aggregate Bond]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1492,12 +1504,12 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="eurpln_m" displayName="eurpln_m" ref="A1:C251" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C251"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="eurpln_m" displayName="eurpln_m" ref="A1:C251" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C251" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Data" queryTableFieldId="1" dataDxfId="12"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="11"/>
-    <tableColumn id="6" uniqueName="6" name="zmiana miesięczna" queryTableFieldId="6" dataDxfId="10" dataCellStyle="Procentowy">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" uniqueName="1" name="Data" queryTableFieldId="1" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" uniqueName="6" name="zmiana miesięczna" queryTableFieldId="6" dataDxfId="29" dataCellStyle="Procentowy">
       <calculatedColumnFormula>eurpln_m[[#This Row],[Zamkniecie]]/B1-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1506,12 +1518,12 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="tbsp_m_1" displayName="tbsp_m_1" ref="A1:C188" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C188"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tbsp_m_1" displayName="tbsp_m_1" ref="A1:C188" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C188" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" uniqueName="1" name="Data" queryTableFieldId="1" dataDxfId="14"/>
-    <tableColumn id="5" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="13"/>
-    <tableColumn id="6" uniqueName="6" name="Kolumna1" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" uniqueName="1" name="Data" queryTableFieldId="1" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" uniqueName="5" name="Zamkniecie" queryTableFieldId="5" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" uniqueName="6" name="Kolumna1" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1813,7 +1825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C414"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -6803,7 +6815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8229,7 +8241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView topLeftCell="A76" workbookViewId="0">
@@ -9439,7 +9451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -12107,7 +12119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D258"/>
   <sheetViews>
     <sheetView topLeftCell="A229" workbookViewId="0">
@@ -15929,7 +15941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18229,10 +18241,12 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="B246" sqref="B246:B250"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -21943,8 +21957,8 @@
       <c r="A248" s="1">
         <v>44681</v>
       </c>
-      <c r="B248" s="10">
-        <v>44652</v>
+      <c r="B248" s="9">
+        <v>44682</v>
       </c>
       <c r="C248" s="2">
         <v>18557.02</v>
@@ -21958,6 +21972,9 @@
       <c r="A249" s="1">
         <v>44712</v>
       </c>
+      <c r="B249" s="10">
+        <v>44713</v>
+      </c>
       <c r="C249" s="2">
         <v>18167.46</v>
       </c>
@@ -21969,6 +21986,9 @@
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>44742</v>
+      </c>
+      <c r="B250" s="9">
+        <v>44743</v>
       </c>
       <c r="C250" s="2">
         <v>17016.89</v>
@@ -21988,10 +22008,10 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A186" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B212"/>
     </sheetView>
   </sheetViews>
@@ -25187,10 +25207,10 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A474" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -31473,7 +31493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView topLeftCell="A224" workbookViewId="0">
@@ -35242,7 +35262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C522"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41528,7 +41548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C522"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47814,7 +47834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C522"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -54100,7 +54120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -58491,11 +58511,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C414"/>
   <sheetViews>
-    <sheetView topLeftCell="A389" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158:A414"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63481,7 +63501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -64703,7 +64723,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C251"/>
   <sheetViews>
     <sheetView topLeftCell="A225" workbookViewId="0">
@@ -67737,7 +67757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>